<commit_message>
i think i am getting the hang of it
</commit_message>
<xml_diff>
--- a/CR_FDIS_3_EGR/CR_FDIS_3_Quality_Reviews_bus.xlsx
+++ b/CR_FDIS_3_EGR/CR_FDIS_3_Quality_Reviews_bus.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$45</definedName>
     <definedName name="elemental_geometric_shape_arm.axis_placement" localSheetId="1">Sheet2!$A$6</definedName>
     <definedName name="elemental_geometric_shape_arm.axis1_placement" localSheetId="1">Sheet2!$A$4</definedName>
     <definedName name="elemental_geometric_shape_arm.axis1_placement.axis" localSheetId="1">Sheet2!$B$4</definedName>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="114">
   <si>
     <t>ap209_multidisciplinary_analysis_and_design</t>
   </si>
@@ -336,15 +336,9 @@
     <t>word mark up done</t>
   </si>
   <si>
-    <t>44 revisions: 33 insertions, 11 deletions</t>
-  </si>
-  <si>
     <t>15 revisions: 12 insertions, 3 deletions</t>
   </si>
   <si>
-    <t>11 revisions: 7 insertions, 4 deletions</t>
-  </si>
-  <si>
     <t>Clause 4</t>
   </si>
   <si>
@@ -352,6 +346,33 @@
   </si>
   <si>
     <t>BS</t>
+  </si>
+  <si>
+    <t>review complete - no change needed</t>
+  </si>
+  <si>
+    <t>8 revisions: 7 insertions, 1 deletion</t>
+  </si>
+  <si>
+    <t>15 revisions: 11 insertions, 4 deletions</t>
+  </si>
+  <si>
+    <t>46 revisions: 35 insertions, 11 deletions</t>
+  </si>
+  <si>
+    <t>13 revisions: 9 insertions, 4 deletions</t>
+  </si>
+  <si>
+    <t>2 revisions: 2 insertions, 0 deletions</t>
+  </si>
+  <si>
+    <t>26 revisions: 21 insertions, 5 deletions</t>
+  </si>
+  <si>
+    <t>3 revisions: 3 insertions</t>
+  </si>
+  <si>
+    <t>9 revisions: 7 insertions, 2 deletions</t>
   </si>
 </sst>
 </file>
@@ -395,7 +416,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -414,6 +435,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -563,7 +590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -572,12 +599,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
@@ -595,6 +616,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1043,7 +1073,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,63 +1086,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" s="16" t="s">
+      <c r="D1" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="E4" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1120,10 +1162,10 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1131,10 +1173,10 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>80</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1144,10 +1186,10 @@
         <v>96</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="12"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1155,237 +1197,241 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="12"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B15" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="C15" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B19" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="C19" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B23" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="C23" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E23" s="12"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>47</v>
+        <v>104</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>85</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>45</v>
+        <v>104</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D25" s="4"/>
-      <c r="E25" s="12"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -1397,10 +1443,10 @@
       <c r="D26" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E26" s="12"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1412,10 +1458,10 @@
       <c r="D27" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E27" s="12"/>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -1427,10 +1473,10 @@
       <c r="D28" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E28" s="12"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1442,10 +1488,10 @@
       <c r="D29" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E29" s="12"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -1457,10 +1503,10 @@
       <c r="D30" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E30" s="12"/>
+      <c r="E30" s="10"/>
     </row>
     <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -1472,10 +1518,10 @@
       <c r="D31" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E31" s="12"/>
+      <c r="E31" s="10"/>
     </row>
     <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -1487,10 +1533,10 @@
       <c r="D32" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="12"/>
+      <c r="E32" s="10"/>
     </row>
     <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -1502,10 +1548,10 @@
       <c r="D33" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E33" s="12"/>
+      <c r="E33" s="10"/>
     </row>
     <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -1517,10 +1563,10 @@
       <c r="D34" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E34" s="12"/>
+      <c r="E34" s="10"/>
     </row>
     <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -1532,10 +1578,10 @@
       <c r="D35" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E35" s="12"/>
+      <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -1547,10 +1593,10 @@
       <c r="D36" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E36" s="12"/>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -1562,10 +1608,10 @@
       <c r="D37" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E37" s="12"/>
+      <c r="E37" s="10"/>
     </row>
     <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -1577,10 +1623,10 @@
       <c r="D38" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E38" s="12"/>
+      <c r="E38" s="10"/>
     </row>
     <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -1592,10 +1638,10 @@
       <c r="D39" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E39" s="12"/>
+      <c r="E39" s="10"/>
     </row>
     <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -1607,10 +1653,10 @@
       <c r="D40" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E40" s="12"/>
+      <c r="E40" s="10"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="6" t="s">
         <v>78</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -1620,10 +1666,10 @@
         <v>96</v>
       </c>
       <c r="D41" s="4"/>
-      <c r="E41" s="12"/>
+      <c r="E41" s="10"/>
     </row>
     <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -1635,10 +1681,10 @@
       <c r="D42" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E42" s="12"/>
+      <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -1650,10 +1696,10 @@
       <c r="D43" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E43" s="12"/>
+      <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -1665,32 +1711,32 @@
       <c r="D44" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E44" s="12"/>
+      <c r="E44" s="10"/>
     </row>
     <row r="45" spans="1:5" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D45" s="11" t="s">
+      <c r="C45" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E45" s="13"/>
+      <c r="E45" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D45">
+  <autoFilter ref="A1:E45">
     <filterColumn colId="2">
       <filters>
         <filter val="BS"/>
       </filters>
     </filterColumn>
-    <sortState ref="A2:D45">
-      <sortCondition descending="1" ref="B1:B45"/>
+    <sortState ref="A2:E25">
+      <sortCondition ref="A1:A45"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
@@ -1716,28 +1762,28 @@
     <hyperlink ref="A28" r:id="rId20" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/swept_solid/sys/cover.htm"/>
     <hyperlink ref="A27" r:id="rId21" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/requirement_management/sys/cover.htm"/>
     <hyperlink ref="A26" r:id="rId22" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/conditional_effectivity/sys/cover.htm"/>
-    <hyperlink ref="A25" r:id="rId23" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/description_assignment/sys/cover.htm"/>
-    <hyperlink ref="A24" r:id="rId24" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/analytical_model/sys/cover.htm"/>
-    <hyperlink ref="A23" r:id="rId25" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/assembly_functional_interface_requirement/sys/cover.htm"/>
-    <hyperlink ref="A22" r:id="rId26" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/assembly_module_with_subassembly/sys/cover.htm"/>
-    <hyperlink ref="A21" r:id="rId27" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/footprint_definition/sys/cover.htm"/>
-    <hyperlink ref="A20" r:id="rId28" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/assembly_physical_interface_requirement/sys/cover.htm"/>
-    <hyperlink ref="A19" r:id="rId29" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/assembly_technology/sys/cover.htm"/>
-    <hyperlink ref="A18" r:id="rId30" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/component_feature/sys/cover.htm"/>
-    <hyperlink ref="A17" r:id="rId31" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/part_template/sys/cover.htm"/>
-    <hyperlink ref="A16" r:id="rId32" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/physical_unit_usage_view/sys/cover.htm"/>
-    <hyperlink ref="A15" r:id="rId33" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/composite_constituent_shape/sys/cover.htm"/>
-    <hyperlink ref="A14" r:id="rId34" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/part_and_zone_laminate_tables/sys/cover.htm"/>
-    <hyperlink ref="A13" r:id="rId35" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/kinematic_motion_representation/sys/cover.htm"/>
-    <hyperlink ref="A12" r:id="rId36" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/process_plan/sys/cover.htm"/>
-    <hyperlink ref="A11" r:id="rId37" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/product_as_individual_assembly_and_test/sys/cover.htm"/>
-    <hyperlink ref="A10" r:id="rId38" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/part_shape/sys/cover.htm"/>
-    <hyperlink ref="A9" r:id="rId39" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/general_design_connectivity/sys/cover.htm"/>
+    <hyperlink ref="A13" r:id="rId23" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/description_assignment/sys/cover.htm"/>
+    <hyperlink ref="A2" r:id="rId24" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/analytical_model/sys/cover.htm"/>
+    <hyperlink ref="A3" r:id="rId25" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/assembly_functional_interface_requirement/sys/cover.htm"/>
+    <hyperlink ref="A4" r:id="rId26" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/assembly_module_with_subassembly/sys/cover.htm"/>
+    <hyperlink ref="A14" r:id="rId27" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/footprint_definition/sys/cover.htm"/>
+    <hyperlink ref="A9" r:id="rId28" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/assembly_physical_interface_requirement/sys/cover.htm"/>
+    <hyperlink ref="A10" r:id="rId29" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/assembly_technology/sys/cover.htm"/>
+    <hyperlink ref="A11" r:id="rId30" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/component_feature/sys/cover.htm"/>
+    <hyperlink ref="A20" r:id="rId31" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/part_template/sys/cover.htm"/>
+    <hyperlink ref="A21" r:id="rId32" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/physical_unit_usage_view/sys/cover.htm"/>
+    <hyperlink ref="A12" r:id="rId33" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/composite_constituent_shape/sys/cover.htm"/>
+    <hyperlink ref="A18" r:id="rId34" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/part_and_zone_laminate_tables/sys/cover.htm"/>
+    <hyperlink ref="A16" r:id="rId35" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/kinematic_motion_representation/sys/cover.htm"/>
+    <hyperlink ref="A22" r:id="rId36" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/process_plan/sys/cover.htm"/>
+    <hyperlink ref="A23" r:id="rId37" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/product_as_individual_assembly_and_test/sys/cover.htm"/>
+    <hyperlink ref="A19" r:id="rId38" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/part_shape/sys/cover.htm"/>
+    <hyperlink ref="A15" r:id="rId39" display="../../../CR_FDIS2/FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/part1000/data/modules/general_design_connectivity/sys/cover.htm"/>
     <hyperlink ref="A41" r:id="rId40" display="../../../FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/iso10303_105/data/resource_docs/kinematics/sys/cover.htm"/>
     <hyperlink ref="A7" r:id="rId41" display="../../../FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/iso10303_41/data/resource_docs/fundamentals_of_product_description_and_support/sys/cover.htm"/>
-    <hyperlink ref="A4" r:id="rId42" display="../../../FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/iso10303_45/data/resource_docs/material_and_other_engineering_properties/sys/cover.htm"/>
-    <hyperlink ref="A3" r:id="rId43" display="../../../FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/iso10303_56/data/resource_docs/state/sys/cover.htm"/>
-    <hyperlink ref="A2" r:id="rId44" display="../../../FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/iso10303_61/data/resource_docs/systems_engineering_representation/sys/cover.htm"/>
+    <hyperlink ref="A17" r:id="rId42" display="../../../FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/iso10303_45/data/resource_docs/material_and_other_engineering_properties/sys/cover.htm"/>
+    <hyperlink ref="A24" r:id="rId43" display="../../../FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/iso10303_56/data/resource_docs/state/sys/cover.htm"/>
+    <hyperlink ref="A25" r:id="rId44" display="../../../FDIS3/CR_FDIS_3_20190220/CR_FDIS_3_20190220/iso10303_61/data/resource_docs/systems_engineering_representation/sys/cover.htm"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId45"/>

</xml_diff>

<commit_message>
more and more i hate this job
</commit_message>
<xml_diff>
--- a/CR_FDIS_3_EGR/CR_FDIS_3_Quality_Reviews_bus.xlsx
+++ b/CR_FDIS_3_EGR/CR_FDIS_3_Quality_Reviews_bus.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="116">
   <si>
     <t>ap209_multidisciplinary_analysis_and_design</t>
   </si>
@@ -373,6 +373,12 @@
   </si>
   <si>
     <t>9 revisions: 7 insertions, 2 deletions</t>
+  </si>
+  <si>
+    <t>1 revision: 1 insertion. 0 deletions</t>
+  </si>
+  <si>
+    <t>43 revisions, 33 insertions, 10 deletions</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1079,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,7 +1252,9 @@
       <c r="D11" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="E11" s="10"/>
+      <c r="E11" s="15" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -1258,7 +1266,9 @@
       <c r="C12" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="19" t="s">
+        <v>115</v>
+      </c>
       <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
one more time i guess
</commit_message>
<xml_diff>
--- a/CR_FDIS_3_EGR/CR_FDIS_3_Quality_Reviews_bus.xlsx
+++ b/CR_FDIS_3_EGR/CR_FDIS_3_Quality_Reviews_bus.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="124">
   <si>
     <t>ap209_multidisciplinary_analysis_and_design</t>
   </si>
@@ -369,9 +369,6 @@
     <t>26 revisions: 21 insertions, 5 deletions</t>
   </si>
   <si>
-    <t>3 revisions: 3 insertions</t>
-  </si>
-  <si>
     <t>9 revisions: 7 insertions, 2 deletions</t>
   </si>
   <si>
@@ -391,13 +388,28 @@
   </si>
   <si>
     <t>11 revisions: 9 insertions, 2 deletions</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>20 revisions: 17 insertions, 3 deletions</t>
+  </si>
+  <si>
+    <t>78 revisions: 43 insertions, 35 deletions</t>
+  </si>
+  <si>
+    <t>3 revisions: 1 insertion, 2 deletions</t>
+  </si>
+  <si>
+    <t>3 revisions: 3 insertions, 0 deletions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,8 +445,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,6 +478,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -608,7 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -643,6 +668,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1091,7 +1117,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,7 +1274,7 @@
         <v>111</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1262,10 +1288,10 @@
         <v>104</v>
       </c>
       <c r="D11" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="15" t="s">
         <v>113</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1279,10 +1305,10 @@
         <v>104</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1296,7 +1322,7 @@
         <v>104</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>110</v>
@@ -1313,7 +1339,7 @@
         <v>104</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>105</v>
@@ -1330,10 +1356,10 @@
         <v>104</v>
       </c>
       <c r="D15" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>117</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1347,9 +1373,11 @@
         <v>104</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="E16" s="10"/>
+        <v>118</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -1361,8 +1389,12 @@
       <c r="C17" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="10"/>
+      <c r="D17" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
@@ -1374,8 +1406,12 @@
       <c r="C18" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="10"/>
+      <c r="D18" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">

</xml_diff>

<commit_message>
to whom it may concern my love
</commit_message>
<xml_diff>
--- a/CR_FDIS_3_EGR/CR_FDIS_3_Quality_Reviews_bus.xlsx
+++ b/CR_FDIS_3_EGR/CR_FDIS_3_Quality_Reviews_bus.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="136">
   <si>
     <t>ap209_multidisciplinary_analysis_and_design</t>
   </si>
@@ -403,6 +403,42 @@
   </si>
   <si>
     <t>3 revisions: 3 insertions, 0 deletions</t>
+  </si>
+  <si>
+    <t>4 revisions: 3 insertions, 1 deletion</t>
+  </si>
+  <si>
+    <t>4 revisions: 2 insertions, 2 deletions</t>
+  </si>
+  <si>
+    <t>27 revisions: 21 insertions, 6 deletions</t>
+  </si>
+  <si>
+    <t>4 revisions: 4 insertions, 0 deletions</t>
+  </si>
+  <si>
+    <t>31 revisions: 23 insertions, 8 deletions</t>
+  </si>
+  <si>
+    <t>7 revisions: 5 insertions, 1 deletions</t>
+  </si>
+  <si>
+    <t>Material_property_definition_schema</t>
+  </si>
+  <si>
+    <t>State_observed_schema</t>
+  </si>
+  <si>
+    <t>State_schema</t>
+  </si>
+  <si>
+    <t>6 revisions: 3 insertions, 3 deletions</t>
+  </si>
+  <si>
+    <t>19 revisions: 11 insertions, 8 deletions</t>
+  </si>
+  <si>
+    <t>10 revisions: 8 insertions, 2 deletions</t>
   </si>
 </sst>
 </file>
@@ -453,7 +489,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -484,6 +520,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -633,7 +675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -669,6 +711,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1114,10 +1158,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,10 +1200,10 @@
       <c r="C2" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="22" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1173,10 +1217,10 @@
       <c r="C3" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="22" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1190,10 +1234,10 @@
       <c r="C4" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="22" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1253,10 +1297,10 @@
       <c r="C9" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="22" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1270,10 +1314,10 @@
       <c r="C10" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="22" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1287,10 +1331,10 @@
       <c r="C11" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="22" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1304,10 +1348,10 @@
       <c r="C12" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="22" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1321,10 +1365,10 @@
       <c r="C13" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="22" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1338,10 +1382,10 @@
       <c r="C14" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="22" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1355,10 +1399,10 @@
       <c r="C15" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="22" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1372,14 +1416,14 @@
       <c r="C16" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="21" t="s">
         <v>118</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>82</v>
       </c>
@@ -1395,8 +1439,11 @@
       <c r="E17" s="20" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>66</v>
       </c>
@@ -1413,7 +1460,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>74</v>
       </c>
@@ -1423,10 +1470,14 @@
       <c r="C19" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>60</v>
       </c>
@@ -1436,10 +1487,14 @@
       <c r="C20" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>62</v>
       </c>
@@ -1449,10 +1504,14 @@
       <c r="C21" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>70</v>
       </c>
@@ -1462,10 +1521,14 @@
       <c r="C22" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>72</v>
       </c>
@@ -1475,10 +1538,14 @@
       <c r="C23" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D23" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>84</v>
       </c>
@@ -1488,10 +1555,20 @@
       <c r="C24" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D24" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" t="s">
+        <v>131</v>
+      </c>
+      <c r="G24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>86</v>
       </c>
@@ -1501,10 +1578,14 @@
       <c r="C25" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>42</v>
       </c>
@@ -1519,7 +1600,7 @@
       </c>
       <c r="E26" s="10"/>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>40</v>
       </c>
@@ -1534,7 +1615,7 @@
       </c>
       <c r="E27" s="10"/>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>38</v>
       </c>
@@ -1549,7 +1630,7 @@
       </c>
       <c r="E28" s="10"/>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>36</v>
       </c>
@@ -1564,7 +1645,7 @@
       </c>
       <c r="E29" s="10"/>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>34</v>
       </c>
@@ -1579,7 +1660,7 @@
       </c>
       <c r="E30" s="10"/>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>32</v>
       </c>
@@ -1594,7 +1675,7 @@
       </c>
       <c r="E31" s="10"/>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>30</v>
       </c>

</xml_diff>